<commit_message>
Enabled TDSE sim in Fourier space
</commit_message>
<xml_diff>
--- a/.config/simulationConfig/latticeSeSim1DConfig/latticeSeSim1DType.csv.xlsx
+++ b/.config/simulationConfig/latticeSeSim1DConfig/latticeSeSim1DType.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Work\MuscleMuseum\.config\simulationConfig\latticeSeSim1DConfig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93462BE6-B2F8-45B0-9A99-A687B13848F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35B3FC5-5825-4779-9CD7-B797B09D2B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,7 +524,7 @@
         <v>10000</v>
       </c>
       <c r="N2">
-        <v>1000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14">

</xml_diff>